<commit_message>
Added a line to motor controller bom, added both libraries, a schematic, and a pcb file
</commit_message>
<xml_diff>
--- a/motor_controller_BOM.xlsx
+++ b/motor_controller_BOM.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmab\Documents\GitHub\MarsRover2019-PCB\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="480" yWindow="110" windowWidth="27800" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="motor_controller_BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="89">
   <si>
     <t>Quantity</t>
   </si>
@@ -275,12 +280,18 @@
   </si>
   <si>
     <t>https://www.digikey.ca/product-detail/en/nexperia-usa-inc/BUK765R3-40E118/1727-7255-1-ND/3672520</t>
+  </si>
+  <si>
+    <t>NEW ITEM</t>
+  </si>
+  <si>
+    <t>FOR TESTING CONFLICT RESOLUTION SKILLS OF GITHUB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -812,6 +823,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -859,7 +873,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -892,9 +906,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -927,6 +958,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1105,18 +1153,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="30.42578125" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" customWidth="1"/>
+    <col min="4" max="4" width="27.1796875" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>81</v>
       </c>
@@ -1142,7 +1190,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>83</v>
       </c>
@@ -1168,7 +1216,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>83</v>
       </c>
@@ -1194,7 +1242,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -1220,7 +1268,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -1246,7 +1294,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>84</v>
       </c>
@@ -1272,7 +1320,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -1298,7 +1346,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -1324,7 +1372,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -1350,7 +1398,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -1376,7 +1424,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>83</v>
       </c>
@@ -1402,7 +1450,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -1428,7 +1476,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>82</v>
       </c>
@@ -1454,7 +1502,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>82</v>
       </c>
@@ -1480,7 +1528,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -1506,7 +1554,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>83</v>
       </c>
@@ -1532,7 +1580,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -1558,7 +1606,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -1584,7 +1632,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B19">
         <v>2</v>
       </c>
@@ -1608,7 +1656,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>83</v>
       </c>
@@ -1634,7 +1682,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -1660,7 +1708,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>83</v>
       </c>
@@ -1686,7 +1734,13 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" t="s">
+        <v>88</v>
+      </c>
       <c r="F23" t="s">
         <v>77</v>
       </c>

</xml_diff>